<commit_message>
Understanding the need for NOSQL data.
</commit_message>
<xml_diff>
--- a/التأليف والتفكيك.xlsx
+++ b/التأليف والتفكيك.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20106\PycharmProjects\Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5BD087-3BBA-46A6-9DD1-5A9E5DDC5B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A8C5FB-62BA-435E-A710-D3C995919CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="هندسة البيانات" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>connect</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>0 cor|cov = linear independence |But| independence is stronger</t>
+  </si>
+  <si>
+    <t>The need for noSQL data</t>
+  </si>
+  <si>
+    <t>مش دايما البيانات تكون على شكل الجداول؛ او يمكن تشكيلها على هيئة جدول؛ عدم القدرة على التمييز بين الكيانات والعلاقات (عكس الجراف)؛ هناك سببين اخرين</t>
   </si>
 </sst>
 </file>
@@ -430,8 +436,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -889,9 +895,13 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+    <row r="15" spans="1:26" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -28533,7 +28543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83229F82-1901-407C-BF29-A7A9E3BD1211}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>